<commit_message>
Updated naming systems, fixed eqcorr2d bugs and added a self-integrated function for calculating match scores in a Megastructure
</commit_message>
<xml_diff>
--- a/crisscross_kit/eqcorr2d/slat_database.xlsx
+++ b/crisscross_kit/eqcorr2d/slat_database.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/crisscross_kit/eqcorr2d/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D897215-1EC5-B445-9B17-66B5ACD0B05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34CBFC-73C0-324F-9984-8A09EBDED447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="double_barrel_type_a" sheetId="1" r:id="rId1"/>
-    <sheet name="double_barrel_type_b" sheetId="4" r:id="rId2"/>
+    <sheet name="double-barrel-A" sheetId="1" r:id="rId1"/>
+    <sheet name="double-barrel-B" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -283,8 +296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="290" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -562,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="216" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>